<commit_message>
removed driver shift times
</commit_message>
<xml_diff>
--- a/master_report.xlsx
+++ b/master_report.xlsx
@@ -1540,7 +1540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1619,16 +1619,6 @@
           <t>Total Errors</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Stow Driver Shift Time (hr)</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Retrieve Driver Shift Time (hr)</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1675,12 +1665,6 @@
       <c r="N2" t="n">
         <v>53</v>
       </c>
-      <c r="O2" t="n">
-        <v>3.801308611666667</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1726,12 +1710,6 @@
       </c>
       <c r="N3" t="n">
         <v>180</v>
-      </c>
-      <c r="O3" t="n">
-        <v>3.182359001666669</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.9681610277777779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>